<commit_message>
parte final do projeto de ACV, com os gráficos de incerteza de h
</commit_message>
<xml_diff>
--- a/B.xlsx
+++ b/B.xlsx
@@ -2,24 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d8f3b2df7dd2c83/UTFPR/ACV - Cassia/Projeto ACV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{6B92FD44-8537-4454-9F47-E005450FD104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D63C1C4-FB33-4945-A1D0-9294DB51F24D}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{31838710-4D0D-4EE8-ABC3-F4B88FE80A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC1AC491-A4A4-49D6-A14D-B3D040BA351B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7307738F-2E62-455F-9F4D-1AD3FBA3DA17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,12 +33,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>col4</t>
-  </si>
-  <si>
-    <t>col5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
   </si>
 </sst>
 </file>
@@ -50,15 +59,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -83,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -102,151 +112,61 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4285F4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="EA4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="FBBC04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="34A853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="FF6D01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,58 +309,108 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F868B3A-C1AB-4D6B-A123-FAAF3926F861}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
+        <v>0.04</v>
+      </c>
+      <c r="C2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C4">
+        <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>-500</v>
+      </c>
+      <c r="C5">
+        <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>-50</v>
-      </c>
-    </row>
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>